<commit_message>
Nadopunjen je ProductBacklog sa novom funkcionalnošću i pripadnim prioritetom
</commit_message>
<xml_diff>
--- a/Dokumentacija/ProductBacklog.xlsx
+++ b/Dokumentacija/ProductBacklog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>LISTA FUNKCIONALNOSTI</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Sprint</t>
+  </si>
+  <si>
+    <t>16.</t>
+  </si>
+  <si>
+    <t>Izmjena korisničkih podataka</t>
   </si>
 </sst>
 </file>
@@ -584,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F19"/>
+  <dimension ref="B3:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F19"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,13 +824,13 @@
         <v>29</v>
       </c>
       <c r="D16" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E16" s="2">
         <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -862,19 +868,36 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2">
+        <v>9</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
         <v>3</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E20" s="1">
         <v>4</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F20" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
U projektnu dokumentaciju je dodano poglavlje Plan iteracija u kojem se nalazi gantogram cjelokupnog projekta. U poglavlju je prikazan sam plan iteracija te potrebni resursi za realizaciju zadataka.
</commit_message>
<xml_diff>
--- a/Dokumentacija/ProductBacklog.xlsx
+++ b/Dokumentacija/ProductBacklog.xlsx
@@ -593,7 +593,7 @@
   <dimension ref="B3:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,13 +756,13 @@
         <v>23</v>
       </c>
       <c r="D12" s="2">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
         <v>6</v>
       </c>
       <c r="F12" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -841,13 +841,13 @@
         <v>28</v>
       </c>
       <c r="D17" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E17" s="2">
         <v>5</v>
       </c>
       <c r="F17" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Napravljene su promjene u projektnoj i tehničkoj dokumentaciji te je dodan novi izmjenjeni Product Backlog te su dodani  dodatni opisi sastanaka
</commit_message>
<xml_diff>
--- a/Dokumentacija/ProductBacklog.xlsx
+++ b/Dokumentacija/ProductBacklog.xlsx
@@ -593,7 +593,7 @@
   <dimension ref="B3:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +756,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
         <v>6</v>
@@ -790,13 +790,13 @@
         <v>26</v>
       </c>
       <c r="D14" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2">
         <v>10</v>
       </c>
       <c r="F14" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>37</v>
       </c>
       <c r="D19" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="2">
         <v>9</v>

</xml_diff>